<commit_message>
- Fixed some spelling errors in item names leading to textures not being found - Text for item names now scale - Drawing cards works and implemented the logic for what is drawn (logic needs tweaking) - Redesigned the Rags to Riches window slightly to better fit everything and increase the card size.
</commit_message>
<xml_diff>
--- a/PVPlayTool/Data/DarkSouls/DaS_Items.xlsx
+++ b/PVPlayTool/Data/DarkSouls/DaS_Items.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Menno\source\repos\PVPlayTool\PVPlayTool\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MennovdHeijden\source\repos\PVPlayTool\PVPlayTool\Data\DarkSouls\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -139,13 +139,13 @@
     <t>tex_DaS_PoisonThrowingKnife.png</t>
   </si>
   <si>
-    <t>tex_DaS_Lloyd'sTalisman.png</t>
-  </si>
-  <si>
     <t>tex_DaS_SilverPendant.png</t>
   </si>
   <si>
     <t>ItemName</t>
+  </si>
+  <si>
+    <t>tex_DaS_LloydsTalisman.png</t>
   </si>
 </sst>
 </file>
@@ -550,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +565,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1162,7 +1162,7 @@
         <v>1</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1176,7 +1176,7 @@
         <v>1</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1190,7 +1190,7 @@
         <v>2</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1204,7 +1204,7 @@
         <v>2</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>